<commit_message>
add data validation on template
</commit_message>
<xml_diff>
--- a/spec/templates/ingest_template.xlsx
+++ b/spec/templates/ingest_template.xlsx
@@ -511,6 +511,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1001">
+      <formula1>"Did not meet inclusion criteria,Procedural/experimenter error,Withdrew/fussy/tired,Outlier"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
remove data validation for field that has no list of expected values
</commit_message>
<xml_diff>
--- a/spec/templates/ingest_template.xlsx
+++ b/spec/templates/ingest_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>disability</t>
-  </si>
-  <si>
-    <t>category</t>
   </si>
 </sst>
 </file>
@@ -511,9 +508,21 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1001">
       <formula1>"Did not meet inclusion criteria,Procedural/experimenter error,Withdrew/fussy/tired,Outlier"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
+      <formula1>"PRIVATE,RESTRICTED,SHARED,PUBLIC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1001">
+      <formula1>"Lab,Home,Classroom,Outdoor,Clinic"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1001">
+      <formula1>"AL,AK,AZ,AR,CA,CO,CT,DE,DC,FL,GA,HI,ID,IL,IN,IA,KS,KY,LA,ME,MT,NE,NV,NH,NJ,NM,NY,NC,ND,OH,OK,OR,MD,MA,MI,MN,MS,MO,PA,RI,SC,SD,TN,TX,UT,VT,VA,WA,WV,WI,WY"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1001">
+      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -522,13 +531,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -560,13 +569,21 @@
         <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
+      <formula1>"American Indian or Alaska Native,Asian,Native Hawaiian or Other Pacific Islander,Black or African American,White,Multiple"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1001">
+      <formula1>"Female,Male"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1001">
+      <formula1>"Not Hispanic or Latino,Hispanic or Latino"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update templates re: clips
</commit_message>
<xml_diff>
--- a/spec/templates/ingest_template.xlsx
+++ b/spec/templates/ingest_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -74,31 +74,19 @@
     <t>file_1</t>
   </si>
   <si>
-    <t>clip_out_start_1</t>
-  </si>
-  <si>
-    <t>clip_out_end_1</t>
-  </si>
-  <si>
-    <t>clip_in_start_1</t>
-  </si>
-  <si>
-    <t>clip_in_end_1</t>
+    <t>clip_out_1</t>
+  </si>
+  <si>
+    <t>clip_in_1</t>
   </si>
   <si>
     <t>file_2</t>
   </si>
   <si>
-    <t>clip_out_start_2</t>
-  </si>
-  <si>
-    <t>clip_out_end_2</t>
-  </si>
-  <si>
-    <t>clip_in_start_2</t>
-  </si>
-  <si>
-    <t>clip_in_end_2</t>
+    <t>clip_out_2</t>
+  </si>
+  <si>
+    <t>clip_in_2</t>
   </si>
   <si>
     <t>birthdate</t>
@@ -451,13 +439,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,18 +517,6 @@
       </c>
       <c r="X1" t="s">
         <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -578,31 +554,31 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" t="s">
-        <v>33</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
clear up bugginess around files and clip times
need to avoid the string "file_" in file related settings :rage1:
</commit_message>
<xml_diff>
--- a/spec/templates/ingest_template.xlsx
+++ b/spec/templates/ingest_template.xlsx
@@ -74,10 +74,10 @@
     <t>file_1</t>
   </si>
   <si>
-    <t>file_name_1</t>
-  </si>
-  <si>
-    <t>clip_out_1</t>
+    <t>fname_1</t>
+  </si>
+  <si>
+    <t>fposition_1clip_out_1</t>
   </si>
   <si>
     <t>clip_in_1</t>
@@ -86,7 +86,7 @@
     <t>file_2</t>
   </si>
   <si>
-    <t>file_name_2</t>
+    <t>fname_2fposition_2</t>
   </si>
   <si>
     <t>clip_out_2</t>

</xml_diff>

<commit_message>
update default ingest templates
</commit_message>
<xml_diff>
--- a/spec/templates/ingest_template.xlsx
+++ b/spec/templates/ingest_template.xlsx
@@ -15,9 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>key</t>
   </si>
   <si>
     <t>date</t>
@@ -445,13 +448,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,23 +532,26 @@
       </c>
       <c r="Z1" t="s">
         <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
       <formula1>"Did not meet inclusion criteria,Procedural/experimenter error,Withdrew/fussy/tired,Outlier"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
-      <formula1>"PRIVATE,RESTRICTED,SHARED,PUBLIC"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1001">
+      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1001">
       <formula1>"Lab,Home,Classroom,Outdoor,Clinic"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1001">
       <formula1>"AL,AK,AZ,AR,CA,CO,CT,DE,DC,FL,GA,HI,ID,IL,IN,IA,KS,KY,LA,ME,MT,NE,NV,NH,NJ,NM,NY,NC,ND,OH,OK,OR,MD,MA,MI,MN,MS,MO,PA,RI,SC,SD,TN,TX,UT,VT,VA,WA,WV,WI,WY"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1001">
       <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
     </dataValidation>
   </dataValidations>
@@ -563,37 +569,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
classification on the file level
also: update templates/fix positioning
</commit_message>
<xml_diff>
--- a/spec/templates/ingest_template.xlsx
+++ b/spec/templates/ingest_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -38,9 +38,6 @@
     <t>exclusion</t>
   </si>
   <si>
-    <t>classification</t>
-  </si>
-  <si>
     <t>setting</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>tasks</t>
   </si>
   <si>
-    <t>position</t>
-  </si>
-  <si>
     <t>transcode_options</t>
   </si>
   <si>
@@ -80,7 +74,13 @@
     <t>fname_1</t>
   </si>
   <si>
-    <t>fposition_1clip_out_1</t>
+    <t>fposition_1</t>
+  </si>
+  <si>
+    <t>fclassification_1</t>
+  </si>
+  <si>
+    <t>clip_out_1</t>
   </si>
   <si>
     <t>clip_in_1</t>
@@ -89,7 +89,13 @@
     <t>file_2</t>
   </si>
   <si>
-    <t>fname_2fposition_2</t>
+    <t>fname_2</t>
+  </si>
+  <si>
+    <t>fposition_2</t>
+  </si>
+  <si>
+    <t>fclassification_2</t>
   </si>
   <si>
     <t>clip_out_2</t>
@@ -448,13 +454,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -536,22 +542,31 @@
       <c r="AA1" t="s">
         <v>26</v>
       </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
       <formula1>"Did not meet inclusion criteria,Procedural/experimenter error,Withdrew/fussy/tired,Outlier"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1001">
+      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AA1001">
+      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1001">
-      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1001">
       <formula1>"Lab,Home,Classroom,Outdoor,Clinic"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1001">
       <formula1>"AL,AK,AZ,AR,CA,CO,CT,DE,DC,FL,GA,HI,ID,IL,IN,IA,KS,KY,LA,ME,MT,NE,NV,NH,NJ,NM,NY,NC,ND,OH,OK,OR,MD,MA,MI,MN,MS,MO,PA,RI,SC,SD,TN,TX,UT,VT,VA,WA,WV,WI,WY"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1001">
       <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
     </dataValidation>
   </dataValidations>
@@ -572,34 +587,34 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
         <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to ingest tools to reflect metric changes in db
- add pregnancy term to ingest script
- update templates and generate those
- update volume.json
</commit_message>
<xml_diff>
--- a/spec/templates/ingest_template.xlsx
+++ b/spec/templates/ingest_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -110,7 +110,7 @@
     <t>age_days</t>
   </si>
   <si>
-    <t>gestational age (weeks)</t>
+    <t>gestational age</t>
   </si>
   <si>
     <t>gender</t>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>disability</t>
+  </si>
+  <si>
+    <t>pregnancy term</t>
   </si>
 </sst>
 </file>
@@ -554,20 +557,20 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
       <formula1>"Did not meet inclusion criteria,Procedural/experimenter error,Withdrew/fussy/tired,Outlier"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1001">
+      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AA1001">
+      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1001">
+      <formula1>"AL,AK,AZ,AR,CA,CO,CT,DE,DC,FL,GA,HI,ID,IL,IN,IA,KS,KY,LA,ME,MT,NE,NV,NH,NJ,NM,NY,NC,ND,OH,OK,OR,MD,MA,MI,MN,MS,MO,PA,RI,SC,SD,TN,TX,UT,VT,VA,WA,WV,WI,WY"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1001">
       <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AA1001">
-      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1001">
       <formula1>"Lab,Home,Classroom,Outdoor,Clinic"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1001">
-      <formula1>"AL,AK,AZ,AR,CA,CO,CT,DE,DC,FL,GA,HI,ID,IL,IN,IA,KS,KY,LA,ME,MT,NE,NV,NH,NJ,NM,NY,NC,ND,OH,OK,OR,MD,MA,MI,MN,MS,MO,PA,RI,SC,SD,TN,TX,UT,VT,VA,WA,WV,WI,WY"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1001">
-      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -576,13 +579,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -616,17 +619,23 @@
       <c r="K1" t="s">
         <v>11</v>
       </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
-      <formula1>"American Indian or Alaska Native,Asian,Native Hawaiian or Other Pacific Islander,Black or African American,White,Multiple"</formula1>
-    </dataValidation>
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1001">
       <formula1>"Female,Male"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
+      <formula1>"American Indian or Alaska Native,Asian,Native Hawaiian or Other Pacific Islander,Black or African American,White,More than one,Unknown or not reported"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1001">
       <formula1>"Not Hispanic or Latino,Hispanic or Latino"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1001">
+      <formula1>"Full term,Preterm"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update fields and templates
</commit_message>
<xml_diff>
--- a/spec/templates/ingest_template.xlsx
+++ b/spec/templates/ingest_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -107,25 +107,25 @@
     <t>birthdate</t>
   </si>
   <si>
-    <t>age_days</t>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>ethnicity</t>
+  </si>
+  <si>
+    <t>disability</t>
   </si>
   <si>
     <t>gestational age</t>
   </si>
   <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>race</t>
-  </si>
-  <si>
-    <t>ethnicity</t>
-  </si>
-  <si>
-    <t>disability</t>
-  </si>
-  <si>
     <t>pregnancy term</t>
+  </si>
+  <si>
+    <t>birth weight</t>
   </si>
 </sst>
 </file>
@@ -579,13 +579,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -593,16 +593,16 @@
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
         <v>33</v>
@@ -611,30 +611,24 @@
         <v>34</v>
       </c>
       <c r="I1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1001">
       <formula1>"Female,Male"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1001">
       <formula1>"American Indian or Alaska Native,Asian,Native Hawaiian or Other Pacific Islander,Black or African American,White,More than one,Unknown or not reported"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1001">
       <formula1>"Not Hispanic or Latino,Hispanic or Latino"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1001">
       <formula1>"Full term,Preterm"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update header text to templates for units
</commit_message>
<xml_diff>
--- a/spec/templates/ingest_template.xlsx
+++ b/spec/templates/ingest_template.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="sessions" sheetId="1" r:id="rId1"/>
-    <sheet name="participants" sheetId="2" r:id="rId2"/>
+    <sheet name="participants" sheetId="1" r:id="rId1"/>
+    <sheet name="sessions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -17,6 +17,36 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
+    <t>participantID</t>
+  </si>
+  <si>
+    <t>birthdate</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>ethnicity</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>disability</t>
+  </si>
+  <si>
+    <t>gestational age (weeks)</t>
+  </si>
+  <si>
+    <t>pregnancy term</t>
+  </si>
+  <si>
+    <t>birth weight (grams)</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
@@ -26,9 +56,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>participantID</t>
-  </si>
-  <si>
     <t>top</t>
   </si>
   <si>
@@ -47,9 +74,6 @@
     <t>state</t>
   </si>
   <si>
-    <t>language</t>
-  </si>
-  <si>
     <t>release</t>
   </si>
   <si>
@@ -102,30 +126,6 @@
   </si>
   <si>
     <t>clip_in_2</t>
-  </si>
-  <si>
-    <t>birthdate</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>race</t>
-  </si>
-  <si>
-    <t>ethnicity</t>
-  </si>
-  <si>
-    <t>disability</t>
-  </si>
-  <si>
-    <t>gestational age</t>
-  </si>
-  <si>
-    <t>pregnancy term</t>
-  </si>
-  <si>
-    <t>birth weight</t>
   </si>
 </sst>
 </file>
@@ -457,13 +457,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,83 +494,20 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
-      <formula1>"Did not meet inclusion criteria,Procedural/experimenter error,Withdrew/fussy/tired,Outlier"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AA1001">
-      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1001">
-      <formula1>"AL,AK,AZ,AR,CA,CO,CT,DE,DC,FL,GA,HI,ID,IL,IN,IA,KS,KY,LA,ME,MT,NE,NV,NH,NJ,NM,NY,NC,ND,OH,OK,OR,MD,MA,MI,MN,MS,MO,PA,RI,SC,SD,TN,TX,UT,VT,VA,WA,WV,WI,WY"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1001">
-      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1001">
-      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1001">
-      <formula1>"Lab,Home,Classroom,Outdoor,Clinic"</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1001">
+      <formula1>"Female,Male"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1001">
+      <formula1>"American Indian or Alaska Native,Asian,Native Hawaiian or Other Pacific Islander,Black or African American,White,More than one,Unknown or not reported"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1001">
+      <formula1>"Not Hispanic or Latino,Hispanic or Latino"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1001">
+      <formula1>"Full term,Preterm"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -579,57 +516,120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="W1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="X1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="Y1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="Z1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
+      <c r="AA1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" t="s">
+      <c r="AB1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" t="s">
+      <c r="AC1" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1001">
-      <formula1>"Female,Male"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1001">
-      <formula1>"American Indian or Alaska Native,Asian,Native Hawaiian or Other Pacific Islander,Black or African American,White,More than one,Unknown or not reported"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1001">
-      <formula1>"Not Hispanic or Latino,Hispanic or Latino"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1001">
-      <formula1>"Full term,Preterm"</formula1>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
+      <formula1>"Did not meet inclusion criteria,Procedural/experimenter error,Withdrew/fussy/tired,Outlier"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AA1001">
+      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1001">
+      <formula1>"AL,AK,AZ,AR,CA,CO,CT,DE,DC,FL,GA,HI,ID,IL,IN,IA,KS,KY,LA,ME,MT,NE,NV,NH,NJ,NM,NY,NC,ND,OH,OK,OR,MD,MA,MI,MN,MS,MO,PA,RI,SC,SD,TN,TX,UT,VT,VA,WA,WV,WI,WY"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1001">
+      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1001">
+      <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1001">
+      <formula1>"Lab,Home,Classroom,Outdoor,Clinic"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update volume.json and templates
</commit_message>
<xml_diff>
--- a/spec/templates/ingest_template.xlsx
+++ b/spec/templates/ingest_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>participantID</t>
   </si>
@@ -38,13 +38,13 @@
     <t>disability</t>
   </si>
   <si>
-    <t>gestational age (weeks)</t>
+    <t>gestational age</t>
   </si>
   <si>
     <t>pregnancy term</t>
   </si>
   <si>
-    <t>birth weight (grams)</t>
+    <t>birth weight</t>
   </si>
   <si>
     <t>name</t>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>tasks</t>
+  </si>
+  <si>
+    <t>task_positions</t>
   </si>
   <si>
     <t>transcode_options</t>
@@ -516,13 +519,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -609,6 +612,9 @@
       </c>
       <c r="AC1" t="s">
         <v>36</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -616,13 +622,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
       <formula1>"Did not meet inclusion criteria,Procedural/experimenter error,Withdrew/fussy/tired,Outlier"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AA1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB1001">
       <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1001">
       <formula1>"AL,AK,AZ,AR,CA,CO,CT,DE,DC,FL,GA,HI,ID,IL,IN,IA,KS,KY,LA,ME,MT,NE,NV,NH,NJ,NM,NY,NC,ND,OH,OK,OR,MD,MA,MI,MN,MS,MO,PA,RI,SC,SD,TN,TX,UT,VT,VA,WA,WV,WI,WY"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1001">
       <formula1>"None,PRIVATE,SHARED,EXCERPTS,PUBLIC"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1001">

</xml_diff>